<commit_message>
pushing family eng map
</commit_message>
<xml_diff>
--- a/shinyapp/data/ListOfResources.xlsx
+++ b/shinyapp/data/ListOfResources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nandinidas/Desktop/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7FF9C1-7B96-3C44-8E1D-C13B745E0D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50277D2-16CA-A441-813A-4102C4F89E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="438">
   <si>
     <t>Resources</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Website</t>
   </si>
   <si>
-    <t>Housing utilities</t>
-  </si>
-  <si>
     <t>1 Harrison Street Southeast, Leesburg, VA 20175</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Referrals, utility and rentassistance</t>
   </si>
   <si>
-    <t>www.loudouncares.org</t>
-  </si>
-  <si>
     <t>Holiday Help</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
   </si>
   <si>
     <t>https://www.lcsj.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family Education </t>
   </si>
   <si>
     <t>Loudoun Nurturing Parenting Program</t>
@@ -218,18 +209,12 @@
     <t>Thanksgiving meal drive-thru</t>
   </si>
   <si>
-    <t>www.loudounhunger.org</t>
-  </si>
-  <si>
     <t>Sterling</t>
   </si>
   <si>
     <t>Tin Cup Fund/Women Giving Back</t>
   </si>
   <si>
-    <t>www.thetincupfund.org</t>
-  </si>
-  <si>
     <t>45945 Center Oak Plaza, Suite 175, Sterling, VA 20166</t>
   </si>
   <si>
@@ -239,9 +224,6 @@
     <t>Thanksgiving meal distribution</t>
   </si>
   <si>
-    <t>www.masefaithfoundation.org</t>
-  </si>
-  <si>
     <t xml:space="preserve">Leesburg </t>
   </si>
   <si>
@@ -258,9 +240,6 @@
   </si>
   <si>
     <t>Toys &amp; gifts</t>
-  </si>
-  <si>
-    <t>www.givingothers.org</t>
   </si>
   <si>
     <t>46175 Westlake Drive, Suite 450
@@ -273,9 +252,6 @@
     <t>ESL classes for families</t>
   </si>
   <si>
-    <t>www.loudounliteracy.org</t>
-  </si>
-  <si>
     <t>21630 Ridgetop Circle, Suite 130
 Sterling, VA 20166</t>
   </si>
@@ -289,12 +265,6 @@
     <t xml:space="preserve">Healthy Families Loudoun program provides intensive, long-term home visiting and case management services that are targeted toward helping families build a foundation for success. Services begin during pregnancy or at birth, and are offered for up to five years, supporting the most critical years in a child’s development. </t>
   </si>
   <si>
-    <t>www.inmed.org</t>
-  </si>
-  <si>
-    <t>Eseentials supply</t>
-  </si>
-  <si>
     <t>INMED Free Family Essentials and COVID Relief</t>
   </si>
   <si>
@@ -320,9 +290,6 @@
     <t>http://library.loudoun.gov</t>
   </si>
   <si>
-    <t>Employment</t>
-  </si>
-  <si>
     <t>8 South Street, SW
 Leesburg, VA 20175</t>
   </si>
@@ -334,9 +301,6 @@
   </si>
   <si>
     <t xml:space="preserve">Resumes, computer classes, interview prep, job search (resources available in Spanish) They also have an office in Sterling. </t>
-  </si>
-  <si>
-    <t>www.crossroadsjobs.org</t>
   </si>
   <si>
     <t>705 East Market Street
@@ -377,9 +341,6 @@
     <t>Distribute diapers</t>
   </si>
   <si>
-    <t>www.novadiaperbank.org</t>
-  </si>
-  <si>
     <t>127 Briarwood Court, Sterling, VA 20164</t>
   </si>
   <si>
@@ -405,9 +366,6 @@
   </si>
   <si>
     <t>Mobile Hope provides support and emergency shelter to youth up to age 24 who are at-risk, precariously housed or homeless and empowers them to become self-sufficient.</t>
-  </si>
-  <si>
-    <t>www.mobile-hope.org</t>
   </si>
   <si>
     <t>Resource</t>
@@ -1272,7 +1230,169 @@
     <t xml:space="preserve">Families </t>
   </si>
   <si>
-    <t>Free</t>
+    <t>Mon - Fri 9 - 5</t>
+  </si>
+  <si>
+    <t>Children, adults</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>All community</t>
+  </si>
+  <si>
+    <t>Adults</t>
+  </si>
+  <si>
+    <t>All communty</t>
+  </si>
+  <si>
+    <t>Mon 1 00 - 2 30</t>
+  </si>
+  <si>
+    <t>All Community</t>
+  </si>
+  <si>
+    <t xml:space="preserve">703-777-2205 </t>
+  </si>
+  <si>
+    <t>Families</t>
+  </si>
+  <si>
+    <t>Mon 10 30 - 11 30</t>
+  </si>
+  <si>
+    <t>Virtual and Interactive learning labs</t>
+  </si>
+  <si>
+    <t>Help pay for childcare</t>
+  </si>
+  <si>
+    <t>Mon - Fri 7 am - 6 pm</t>
+  </si>
+  <si>
+    <t> Program's Website</t>
+  </si>
+  <si>
+    <t>Women, Infants and Children (WIC)Women, Infants and Children (WIC)</t>
+  </si>
+  <si>
+    <t>Government Food benefits</t>
+  </si>
+  <si>
+    <t>Mon - Fri 8 - 4 30</t>
+  </si>
+  <si>
+    <t>Program's Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon - Fri 9 30 - 5 30 </t>
+  </si>
+  <si>
+    <t>Free Family Essentials and COVID ReliefFree Family Essentials and COVID Relief</t>
+  </si>
+  <si>
+    <t>2 Pidgeon Hill Drive, Sterling, VA 20165</t>
+  </si>
+  <si>
+    <t>Mon - Fri 8 -5</t>
+  </si>
+  <si>
+    <t>Family Literacy Program</t>
+  </si>
+  <si>
+    <t>Reading sessions, book clubs</t>
+  </si>
+  <si>
+    <t>7611 Little River Turnpike, Annandale, VA 22003</t>
+  </si>
+  <si>
+    <t>Helps employ people with disabilites</t>
+  </si>
+  <si>
+    <t>Career services, Job Coaching</t>
+  </si>
+  <si>
+    <t>4713 Wisconsin Avenue Northwest, Washington, DC 20016</t>
+  </si>
+  <si>
+    <t>Veteran Services</t>
+  </si>
+  <si>
+    <t>Homeless prevention for veterans, case management, Employment services and job placement</t>
+  </si>
+  <si>
+    <t>750 Miller Drive Southeast, Leesburg, VA 20175</t>
+  </si>
+  <si>
+    <t>Employment Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Resume preparation, job placement  </t>
+  </si>
+  <si>
+    <t>Mon 8 - 5</t>
+  </si>
+  <si>
+    <t>11150 Fairfax Boulevard, Fairfax, VA 22030</t>
+  </si>
+  <si>
+    <t>Vocational Rehabilition Services</t>
+  </si>
+  <si>
+    <t>Job placement, Adaptive equipment for training</t>
+  </si>
+  <si>
+    <t>1010 Grandin Avenue, Rockville, MD 20851</t>
+  </si>
+  <si>
+    <t>Employment Help</t>
+  </si>
+  <si>
+    <t>Employment Programs</t>
+  </si>
+  <si>
+    <t>Strenghts assessment, Skills development, Supported Employment</t>
+  </si>
+  <si>
+    <t>The Gift of Sound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Education </t>
+  </si>
+  <si>
+    <t>Essentials supply</t>
+  </si>
+  <si>
+    <t>https://www.loudounliteracy.org</t>
+  </si>
+  <si>
+    <t>https://www.crossroadsjobs.org</t>
+  </si>
+  <si>
+    <t>https://www.inmed.org</t>
+  </si>
+  <si>
+    <t>https://www.loudounhunger.org</t>
+  </si>
+  <si>
+    <t>https://www.thetincupfund.org</t>
+  </si>
+  <si>
+    <t>https://www.masefaithfoundation.org</t>
+  </si>
+  <si>
+    <t>https://www.givingothers.org</t>
+  </si>
+  <si>
+    <t>https://www.loudouncares.org</t>
+  </si>
+  <si>
+    <t>https://www.mobile-hope.org</t>
+  </si>
+  <si>
+    <t>https://www.novadiaperbank.org</t>
   </si>
 </sst>
 </file>
@@ -1834,10 +1954,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M32"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1852,7 +1973,7 @@
     <col min="8" max="8" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1863,7 +1984,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>397</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1880,387 +2001,404 @@
       <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="16" customHeight="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="19"/>
+        <v>426</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>39.114031563604698</v>
+        <v>39.114541830958999</v>
       </c>
       <c r="F2">
-        <v>-77.562010044107197</v>
+        <v>-77.562813165687601</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>13</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="J2"/>
+      <c r="K2"/>
       <c r="L2" t="s">
-        <v>395</v>
-      </c>
-      <c r="M2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>383</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16" customHeight="1">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="19"/>
+        <v>426</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>391</v>
+      </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>39.113352641326003</v>
-      </c>
-      <c r="F3">
-        <v>-77.566373372942493</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="E3" s="16">
+        <v>39.034731000000001</v>
+      </c>
+      <c r="F3" s="16">
+        <v>-77.401696999999999</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="L3" t="s">
+        <v>381</v>
+      </c>
+      <c r="M3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="43">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="19"/>
+        <v>422</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4">
-        <v>39.098255610555597</v>
-      </c>
-      <c r="F4">
-        <v>-77.540925888283695</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="E4" s="16">
+        <v>39.112604699999999</v>
+      </c>
+      <c r="F4" s="16">
+        <v>-77.566093300000006</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="L4" t="s">
+        <v>393</v>
+      </c>
+      <c r="M4" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="48">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
+        <v>422</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>88</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5">
-        <v>39.098255610555597</v>
-      </c>
-      <c r="F5">
-        <v>-77.540925888283695</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>22</v>
+      <c r="E5" s="16">
+        <v>39.114444800000001</v>
+      </c>
+      <c r="F5" s="16">
+        <v>-77.541544200000004</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="20"/>
+        <v>422</v>
+      </c>
+      <c r="B6" t="s">
+        <v>408</v>
+      </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>38.969747395867799</v>
+        <v>38.832196635409097</v>
       </c>
       <c r="F6">
-        <v>-77.736489240505904</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>29</v>
+        <v>-77.208832344596601</v>
+      </c>
+      <c r="G6" t="s">
+        <v>409</v>
+      </c>
+      <c r="H6" t="s">
+        <v>410</v>
+      </c>
+      <c r="L6" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
+        <v>422</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>411</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>39.114541830958999</v>
+        <v>38.951633156260399</v>
       </c>
       <c r="F7">
-        <v>-77.562813165687601</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>35</v>
+        <v>-77.080605088769104</v>
+      </c>
+      <c r="G7" t="s">
+        <v>412</v>
+      </c>
+      <c r="H7" t="s">
+        <v>413</v>
+      </c>
+      <c r="L7" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
+        <v>422</v>
+      </c>
+      <c r="B8" t="s">
+        <v>414</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>39.114541830958999</v>
+        <v>39.082949325821097</v>
       </c>
       <c r="F8">
-        <v>-77.562813165687601</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>35</v>
+        <v>-77.554981328767099</v>
+      </c>
+      <c r="G8" t="s">
+        <v>415</v>
+      </c>
+      <c r="H8" t="s">
+        <v>416</v>
+      </c>
+      <c r="L8" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
+        <v>422</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>418</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>39.114541830958999</v>
+        <v>38.8558681151993</v>
       </c>
       <c r="F9">
-        <v>-77.562813165687601</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>35</v>
+        <v>-77.329504031101493</v>
+      </c>
+      <c r="G9" t="s">
+        <v>419</v>
+      </c>
+      <c r="H9" t="s">
+        <v>420</v>
+      </c>
+      <c r="L9" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
+        <v>422</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>421</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>39.114541830958999</v>
+        <v>39.080275146794399</v>
       </c>
       <c r="F10">
-        <v>-77.562813165687601</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>-77.132470117600604</v>
+      </c>
+      <c r="G10" t="s">
+        <v>423</v>
+      </c>
+      <c r="H10" t="s">
+        <v>424</v>
+      </c>
+      <c r="L10" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="57">
       <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>31</v>
+        <v>427</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11">
-        <v>39.114541830958999</v>
-      </c>
-      <c r="F11">
-        <v>-77.562813165687601</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>35</v>
+      <c r="E11" s="16">
+        <v>39.027190400000002</v>
+      </c>
+      <c r="F11" s="16">
+        <v>-77.408413899999999</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="L11" t="s">
+        <v>381</v>
+      </c>
+      <c r="M11" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
+        <v>427</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>39.114541830958999</v>
+        <v>39.0272778503046</v>
       </c>
       <c r="F12">
-        <v>-77.562813165687601</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>35</v>
+        <v>-77.408538244590801</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="I12" t="s">
+        <v>401</v>
+      </c>
+      <c r="L12" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="20"/>
+        <v>427</v>
+      </c>
+      <c r="B13" t="s">
+        <v>404</v>
+      </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>39.078257453225497</v>
+        <v>39.038094714586698</v>
       </c>
       <c r="F13">
-        <v>-77.550329003624995</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>52</v>
+        <v>-77.413299888285096</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>425</v>
+      </c>
+      <c r="L13" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="19"/>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>39.130864660428202</v>
+        <v>39.098255610555597</v>
       </c>
       <c r="F14">
-        <v>-77.569871180350702</v>
+        <v>-77.540925888283695</v>
       </c>
       <c r="G14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" t="s">
+        <v>381</v>
+      </c>
+      <c r="M14" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="32">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="36" customHeight="1">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15">
@@ -2273,21 +2411,27 @@
         <v>-77.555034971164702</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>56</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="L15" t="s">
+        <v>389</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="36" customHeight="1">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2299,21 +2443,21 @@
         <v>-77.426874346022601</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>59</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>64</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2325,21 +2469,21 @@
         <v>-77.487399999999994</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>61</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2351,21 +2495,21 @@
         <v>-77.564637416464194</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2377,384 +2521,781 @@
         <v>-77.469991169314895</v>
       </c>
       <c r="G19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="L19" t="s">
+        <v>381</v>
+      </c>
+      <c r="M19" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="16">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>39.114031563604698</v>
+      </c>
+      <c r="F20">
+        <v>-77.562010044107197</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" t="s">
+        <v>381</v>
+      </c>
+      <c r="M20" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="29" customHeight="1">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>39.113352641326003</v>
+      </c>
+      <c r="F21">
+        <v>-77.566373372942493</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="L21" t="s">
+        <v>383</v>
+      </c>
+      <c r="M21" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="32" customHeight="1">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>39.098255610555597</v>
+      </c>
+      <c r="F22">
+        <v>-77.540925888283695</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" t="s">
+        <v>381</v>
+      </c>
+      <c r="M22" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="32" customHeight="1">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>38.969747395867799</v>
+      </c>
+      <c r="F23">
+        <v>-77.736489240505904</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="32" customHeight="1">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>39.078257453225497</v>
+      </c>
+      <c r="F24">
+        <v>-77.550329003624995</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="26" customHeight="1">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
         <v>72</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="29" customHeight="1">
-      <c r="A20" t="s">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="16">
+        <v>39.027190400000002</v>
+      </c>
+      <c r="F25" s="16">
+        <v>-77.408413899999999</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="L25" t="s">
+        <v>381</v>
+      </c>
+      <c r="M25" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="17">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>39.110133927921197</v>
+      </c>
+      <c r="F26">
+        <v>-77.556985799931297</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" s="16">
-        <v>39.034731000000001</v>
-      </c>
-      <c r="F20" s="16">
-        <v>-77.401696999999999</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="32" customHeight="1">
-      <c r="A21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" s="16">
-        <v>39.027190400000002</v>
-      </c>
-      <c r="F21" s="16">
-        <v>-77.408413899999999</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="32" customHeight="1">
-      <c r="A22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" s="16">
-        <v>39.027190400000002</v>
-      </c>
-      <c r="F22" s="16">
-        <v>-77.408413899999999</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="32" customHeight="1">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" s="16">
-        <v>39.027190400000002</v>
-      </c>
-      <c r="F23" s="16">
-        <v>-77.408413899999999</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="26" customHeight="1">
-      <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="16">
-        <v>38.989677999999998</v>
-      </c>
-      <c r="F24" s="16">
-        <v>-77.427879000000004</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="43">
-      <c r="A25" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" s="16">
-        <v>39.112604699999999</v>
-      </c>
-      <c r="F25" s="16">
-        <v>-77.566093300000006</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="48">
-      <c r="A26" t="s">
-        <v>93</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="21" t="s">
+      <c r="B27" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>39.114541830958999</v>
+      </c>
+      <c r="F27">
+        <v>-77.562813165687601</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L27" t="s">
+        <v>383</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="21"/>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>39.130864660428202</v>
+      </c>
+      <c r="F28">
+        <v>-77.569871180350702</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" s="16">
-        <v>39.114444800000001</v>
-      </c>
-      <c r="F26" s="16">
-        <v>-77.541544200000004</v>
-      </c>
-      <c r="G26" s="16" t="s">
+      <c r="C29" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="H29" s="18" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="28" t="s">
+      <c r="I29" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27" s="16">
-        <v>39.052760999999997</v>
-      </c>
-      <c r="F27" s="16">
-        <v>-77.360856999999996</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="32">
-      <c r="A28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28" s="16">
-        <v>39.048402699999997</v>
-      </c>
-      <c r="F28" s="16">
-        <v>-77.394760070000004</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="16">
-      <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29" s="16">
-        <v>39.048402699999997</v>
-      </c>
-      <c r="F29" s="16">
-        <v>-77.394760070000004</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="L29" t="s">
+        <v>383</v>
+      </c>
+      <c r="M29" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>114</v>
+      <c r="B30" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
       </c>
       <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="17">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>39.114541830958999</v>
+      </c>
+      <c r="F30">
+        <v>-77.562813165687601</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L30" t="s">
+        <v>383</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="C31" s="23"/>
+        <v>39</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>39.110133927921197</v>
+        <v>39.114541830958999</v>
       </c>
       <c r="F31">
-        <v>-77.556985799931297</v>
+        <v>-77.562813165687601</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="H31" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="32">
+        <v>42</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" t="s">
+        <v>383</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>75</v>
+        <v>39</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>39.114541830958999</v>
+      </c>
+      <c r="F32">
+        <v>-77.562813165687601</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L32" t="s">
+        <v>383</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="113">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="16">
+        <v>39.027190400000002</v>
+      </c>
+      <c r="F33" s="16">
+        <v>-77.408413899999999</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="L33" t="s">
+        <v>381</v>
+      </c>
+      <c r="M33" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="32">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="16">
+        <v>38.989677999999998</v>
+      </c>
+      <c r="F34" s="16">
+        <v>-77.427879000000004</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L34" t="s">
+        <v>381</v>
+      </c>
+      <c r="M34" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" s="16">
+        <v>39.052760999999997</v>
+      </c>
+      <c r="F35" s="16">
+        <v>-77.360856999999996</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="32">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" s="16">
+        <v>39.007011852297097</v>
+      </c>
+      <c r="F36" s="16">
+        <v>-77.436550055823901</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="16">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" s="16">
+        <v>39.048402699999997</v>
+      </c>
+      <c r="F37" s="16">
+        <v>-77.394760070000004</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="16">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="L38" t="s">
+        <v>396</v>
+      </c>
+      <c r="M38" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>39.050746308970503</v>
+      </c>
+      <c r="F39">
+        <v>-77.435347059931004</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="I39" t="s">
+        <v>401</v>
+      </c>
+      <c r="L39" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>38.832196635409097</v>
+      </c>
+      <c r="F40">
+        <v>-77.208832344596601</v>
+      </c>
+      <c r="G40" t="s">
+        <v>406</v>
+      </c>
+      <c r="H40" t="s">
+        <v>407</v>
+      </c>
+      <c r="L40" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>39.114541830958999</v>
+      </c>
+      <c r="F41">
+        <v>-77.562813165687601</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L41" t="s">
+        <v>383</v>
+      </c>
+      <c r="M41" s="11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>39.114541830958999</v>
+      </c>
+      <c r="F42">
+        <v>-77.562813165687601</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L42" t="s">
+        <v>383</v>
+      </c>
+      <c r="M42" s="11" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M42">
+    <sortCondition ref="A2:A42"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{1ACAA4FC-4003-6442-A134-E687764C13E7}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{7CB9EF18-8E82-B448-8B17-57970AE6C3A1}"/>
-    <hyperlink ref="I5" r:id="rId3" xr:uid="{2DD12525-FF1F-5246-9C11-C9B772841256}"/>
-    <hyperlink ref="I9" r:id="rId4" xr:uid="{57F31AA9-2FE1-9B41-9FDF-1E25C7C0913F}"/>
-    <hyperlink ref="I13" r:id="rId5" xr:uid="{3566ACF5-23AA-8249-9262-8EBDD2677182}"/>
-    <hyperlink ref="I14" r:id="rId6" xr:uid="{2E6A4286-C6B3-4E45-BEA5-0B0C3486CF27}"/>
+    <hyperlink ref="I20" r:id="rId1" xr:uid="{1ACAA4FC-4003-6442-A134-E687764C13E7}"/>
+    <hyperlink ref="I21" r:id="rId2" xr:uid="{7CB9EF18-8E82-B448-8B17-57970AE6C3A1}"/>
+    <hyperlink ref="I22" r:id="rId3" xr:uid="{2DD12525-FF1F-5246-9C11-C9B772841256}"/>
+    <hyperlink ref="I27" r:id="rId4" xr:uid="{57F31AA9-2FE1-9B41-9FDF-1E25C7C0913F}"/>
+    <hyperlink ref="I24" r:id="rId5" xr:uid="{3566ACF5-23AA-8249-9262-8EBDD2677182}"/>
+    <hyperlink ref="I28" r:id="rId6" xr:uid="{2E6A4286-C6B3-4E45-BEA5-0B0C3486CF27}"/>
     <hyperlink ref="I15" r:id="rId7" xr:uid="{4CC9BB40-F8FC-A74F-88C0-C33F10D40BC4}"/>
     <hyperlink ref="I16" r:id="rId8" xr:uid="{F4E35388-1758-CD45-9426-D6ADA75B3396}"/>
     <hyperlink ref="I17" r:id="rId9" xr:uid="{DD11ED06-4AA8-4F40-89EC-B821C80F5DFC}"/>
     <hyperlink ref="I19" r:id="rId10" xr:uid="{028CAE33-F8D2-C24D-A3A9-32DE7B9BF2B1}"/>
-    <hyperlink ref="I20" r:id="rId11" display="http://www.loudounliteracy.org/" xr:uid="{0EADE2EC-DBB6-CC4D-818E-16B3DE7A090C}"/>
-    <hyperlink ref="I24" r:id="rId12" display="http://library.loudoun.gov/" xr:uid="{27323F75-8BF5-4947-B758-33F1B0EAF27F}"/>
-    <hyperlink ref="I25" r:id="rId13" display="http://www.crossroadsjobs.org/" xr:uid="{DB176319-F261-D94D-AF5A-882EEFA33FD4}"/>
-    <hyperlink ref="I26" r:id="rId14" xr:uid="{CB4E4518-210C-D942-81D9-25441678AB1F}"/>
-    <hyperlink ref="I27" r:id="rId15" display="http://www.thetincupfund.org/" xr:uid="{39D49696-4851-2D44-9725-A82C7E0FD0A4}"/>
-    <hyperlink ref="I29" r:id="rId16" display="http://www.novadiaperbank.org/" xr:uid="{B312972F-5829-7244-94F4-CAC89EE6D79A}"/>
-    <hyperlink ref="I30" r:id="rId17" xr:uid="{FADDD140-59C4-1F45-A48A-CB795E3B5FC8}"/>
-    <hyperlink ref="I31" r:id="rId18" xr:uid="{AED8550B-15DD-0B47-98EA-81894F4C9327}"/>
-    <hyperlink ref="I4" r:id="rId19" xr:uid="{2ACB2BE1-DF62-C642-B69C-A68BD2483E64}"/>
-    <hyperlink ref="I8" r:id="rId20" xr:uid="{DDA80801-F94F-BF4F-AFEA-D2370F4DF138}"/>
-    <hyperlink ref="I7" r:id="rId21" xr:uid="{087C169C-015B-D240-AA1F-D6F4BAA0D66B}"/>
-    <hyperlink ref="I12" r:id="rId22" xr:uid="{A89A6E34-A995-934D-B839-1BF48A35A95A}"/>
-    <hyperlink ref="I11" r:id="rId23" xr:uid="{17D17ADA-E445-FF40-BE09-2ED185DC2407}"/>
-    <hyperlink ref="I10" r:id="rId24" xr:uid="{73DBB6FD-EF8A-A848-93A3-9351844975C5}"/>
-    <hyperlink ref="I23" r:id="rId25" display="http://www.inmed.org/" xr:uid="{74AC6C11-515E-DF4F-A58C-C4CB028E0D49}"/>
-    <hyperlink ref="I21" r:id="rId26" display="http://www.inmed.org/" xr:uid="{9CA30D57-EC2C-6F45-A659-32CDDC28FFDB}"/>
-    <hyperlink ref="I22" r:id="rId27" display="http://www.inmed.org/" xr:uid="{D9A26D17-B3B0-4743-8F38-74551014F626}"/>
-    <hyperlink ref="I28" r:id="rId28" display="http://www.novadiaperbank.org/" xr:uid="{CF1905A0-DCCA-8346-8546-D4D62FB8B10D}"/>
+    <hyperlink ref="I3" r:id="rId11" xr:uid="{0EADE2EC-DBB6-CC4D-818E-16B3DE7A090C}"/>
+    <hyperlink ref="I34" r:id="rId12" display="http://library.loudoun.gov/" xr:uid="{27323F75-8BF5-4947-B758-33F1B0EAF27F}"/>
+    <hyperlink ref="I4" r:id="rId13" xr:uid="{DB176319-F261-D94D-AF5A-882EEFA33FD4}"/>
+    <hyperlink ref="I5" r:id="rId14" xr:uid="{CB4E4518-210C-D942-81D9-25441678AB1F}"/>
+    <hyperlink ref="I35" r:id="rId15" xr:uid="{39D49696-4851-2D44-9725-A82C7E0FD0A4}"/>
+    <hyperlink ref="I37" r:id="rId16" xr:uid="{B312972F-5829-7244-94F4-CAC89EE6D79A}"/>
+    <hyperlink ref="I29" r:id="rId17" xr:uid="{FADDD140-59C4-1F45-A48A-CB795E3B5FC8}"/>
+    <hyperlink ref="I26" r:id="rId18" xr:uid="{AED8550B-15DD-0B47-98EA-81894F4C9327}"/>
+    <hyperlink ref="I14" r:id="rId19" xr:uid="{2ACB2BE1-DF62-C642-B69C-A68BD2483E64}"/>
+    <hyperlink ref="I2" r:id="rId20" xr:uid="{DDA80801-F94F-BF4F-AFEA-D2370F4DF138}"/>
+    <hyperlink ref="I32" r:id="rId21" xr:uid="{A89A6E34-A995-934D-B839-1BF48A35A95A}"/>
+    <hyperlink ref="I31" r:id="rId22" xr:uid="{17D17ADA-E445-FF40-BE09-2ED185DC2407}"/>
+    <hyperlink ref="I30" r:id="rId23" xr:uid="{73DBB6FD-EF8A-A848-93A3-9351844975C5}"/>
+    <hyperlink ref="I25" r:id="rId24" xr:uid="{74AC6C11-515E-DF4F-A58C-C4CB028E0D49}"/>
+    <hyperlink ref="I33" r:id="rId25" xr:uid="{9CA30D57-EC2C-6F45-A659-32CDDC28FFDB}"/>
+    <hyperlink ref="I11" r:id="rId26" xr:uid="{D9A26D17-B3B0-4743-8F38-74551014F626}"/>
+    <hyperlink ref="I36" r:id="rId27" xr:uid="{CF1905A0-DCCA-8346-8546-D4D62FB8B10D}"/>
+    <hyperlink ref="I38" r:id="rId28" location="1597350518575-7190bf4e-0db4" display="https://www.ymcadc.org/learninglabs/ - 1597350518575-7190bf4e-0db4" xr:uid="{F58BDD75-D52A-42B0-9AE2-05C40AA46ACA}"/>
+    <hyperlink ref="B39" r:id="rId29" display="https://www.google.com/maps/?q=45201+Research+Place,+Ashburn,+VA+20147/" xr:uid="{E022ABD6-6134-46B5-AF89-A0A58BBA3C64}"/>
+    <hyperlink ref="B12" r:id="rId30" display="https://www.google.com/maps/?q=21630+Ridgetop+Circle,+Sterling,+VA+20166/" xr:uid="{ED2A81B6-BD19-4AB2-9A9A-C3F66968965D}"/>
+    <hyperlink ref="B40" r:id="rId31" display="https://www.google.com/maps/?q=7611+Little+River+Turnpike,+Annandale,+VA+22003/" xr:uid="{D6BF060D-51D9-48AE-A822-607C72B3923A}"/>
+    <hyperlink ref="B7" r:id="rId32" display="https://www.google.com/maps/?q=4713+Wisconsin+Avenue+Northwest,+Washington,+DC+20016/" xr:uid="{BF2D07F9-CA87-4772-AF7E-94EBCD1181EA}"/>
+    <hyperlink ref="B9" r:id="rId33" display="https://www.google.com/maps/?q=11150+Fairfax+Boulevard,+Fairfax,+VA+22030/" xr:uid="{939A2862-5411-403B-AB6E-690F26CCCDFB}"/>
+    <hyperlink ref="B10" r:id="rId34" display="https://www.google.com/maps/?q=1010+Grandin+Avenue,+Rockville,+MD+20851/" xr:uid="{65F7C51D-4074-4D09-9D6A-5E7259C39EEA}"/>
+    <hyperlink ref="I42" r:id="rId35" xr:uid="{69A3953A-7F4F-7D40-B28D-1DD3E6D0F44C}"/>
+    <hyperlink ref="I41" r:id="rId36" xr:uid="{087C169C-015B-D240-AA1F-D6F4BAA0D66B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
 
@@ -2775,13 +3316,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2798,10 +3339,10 @@
     </row>
     <row r="2" spans="1:7" ht="80">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2813,18 +3354,18 @@
         <v>-77.382812299999998</v>
       </c>
       <c r="F2" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2836,18 +3377,18 @@
         <v>-77.408413899999999</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="48">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2859,18 +3400,18 @@
         <v>-77.392816800000006</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2882,18 +3423,18 @@
         <v>-77.532362000000006</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="G5" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2905,77 +3446,77 @@
         <v>-77.2368594</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="G6" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="G7" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="G8" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="G9" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G10" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2987,18 +3528,18 @@
         <v>-77.379435099999995</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="G11" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -3010,18 +3551,18 @@
         <v>-77.379055100000002</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="G12" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -3033,18 +3574,18 @@
         <v>-77.497559300000006</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="G13" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -3056,18 +3597,18 @@
         <v>-77.252410999999995</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="G14" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -3079,18 +3620,18 @@
         <v>-77.435420399999998</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="G15" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -3102,18 +3643,18 @@
         <v>-77.426618700000006</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="G16" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -3125,18 +3666,18 @@
         <v>-77.392816800000006</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="G17" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3148,18 +3689,18 @@
         <v>-77.457413900000006</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="G18" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -3171,18 +3712,18 @@
         <v>-77.715368299999994</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="G19" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -3194,18 +3735,18 @@
         <v>-77.497559300000006</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="G20" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -3217,18 +3758,18 @@
         <v>-77.3661089</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="G21" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -3240,18 +3781,18 @@
         <v>-77.541145999999998</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="G22" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -3263,18 +3804,18 @@
         <v>-77.555361099999999</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="G23" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -3286,18 +3827,18 @@
         <v>-77.715578399999998</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="G24" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3309,18 +3850,18 @@
         <v>-77.408413899999999</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="G25" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3332,18 +3873,18 @@
         <v>-77.448892999999998</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="G26" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3355,18 +3896,18 @@
         <v>-77.448892999999998</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="G27" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B28" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3378,18 +3919,18 @@
         <v>-77.395377400000001</v>
       </c>
       <c r="F28" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="G28" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B29" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3401,18 +3942,18 @@
         <v>-77.380240000000001</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="G29" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B30" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3424,18 +3965,18 @@
         <v>-77.380240000000001</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="G30" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3447,18 +3988,18 @@
         <v>-77.466695999999999</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G31" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B32" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3470,18 +4011,18 @@
         <v>-77.536346435546804</v>
       </c>
       <c r="F32" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="G32" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3493,18 +4034,18 @@
         <v>-77.542959999999994</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="G33" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B34" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3516,18 +4057,18 @@
         <v>-77.236164000000002</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="G34" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B35" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3539,18 +4080,18 @@
         <v>-77.413260300000005</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G35" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B36" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3562,18 +4103,18 @@
         <v>-77.435420399999998</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G36" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -3585,18 +4126,18 @@
         <v>-77.541605000000004</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="G37" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -3608,18 +4149,18 @@
         <v>-77.305379000000002</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="G38" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B39" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -3631,18 +4172,18 @@
         <v>-77.715578399999998</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="G39" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B40" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -3654,18 +4195,18 @@
         <v>-77.715578399999998</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="G40" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -3677,18 +4218,18 @@
         <v>-77.457563199999996</v>
       </c>
       <c r="F41" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="G41" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -3700,18 +4241,18 @@
         <v>-77.375699499999996</v>
       </c>
       <c r="F42" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="G42" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3723,18 +4264,18 @@
         <v>-77.435420399999998</v>
       </c>
       <c r="F43" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G43" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -3746,18 +4287,18 @@
         <v>-77.397841900000003</v>
       </c>
       <c r="F44" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="G44" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B45" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3769,18 +4310,18 @@
         <v>-77.478551199999998</v>
       </c>
       <c r="F45" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G45" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B46" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -3792,18 +4333,18 @@
         <v>-77.564622499999999</v>
       </c>
       <c r="F46" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="G46" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="B47" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -3815,18 +4356,18 @@
         <v>-77.222458900000007</v>
       </c>
       <c r="F47" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="G47" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B48" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -3838,18 +4379,18 @@
         <v>-77.235717500000007</v>
       </c>
       <c r="F48" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="G48" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B49" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -3861,18 +4402,18 @@
         <v>-77.486551599999999</v>
       </c>
       <c r="F49" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="G49" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B50" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -3884,18 +4425,18 @@
         <v>-77.399366999999998</v>
       </c>
       <c r="F50" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="G50" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B51" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -3907,18 +4448,18 @@
         <v>-77.399366999999998</v>
       </c>
       <c r="F51" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="G51" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="B52" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -3930,18 +4471,18 @@
         <v>-77.399366999999998</v>
       </c>
       <c r="F52" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="G52" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -3953,18 +4494,18 @@
         <v>-77.393666100000004</v>
       </c>
       <c r="F53" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="G53" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -3976,18 +4517,18 @@
         <v>-77.191912599999995</v>
       </c>
       <c r="F54" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="G54" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3999,18 +4540,18 @@
         <v>-77.103767599999998</v>
       </c>
       <c r="F55" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="G55" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -4022,18 +4563,18 @@
         <v>-77.448892999999998</v>
       </c>
       <c r="F56" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="G56" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -4045,18 +4586,18 @@
         <v>-77.4392</v>
       </c>
       <c r="F57" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="G57" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -4068,18 +4609,18 @@
         <v>-77.407484600000004</v>
       </c>
       <c r="F58" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G58" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -4091,18 +4632,18 @@
         <v>-77.412748199999996</v>
       </c>
       <c r="F59" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="G59" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -4114,18 +4655,18 @@
         <v>-77.389666000000005</v>
       </c>
       <c r="F60" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="G60" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -4137,18 +4678,18 @@
         <v>-77.347973999999994</v>
       </c>
       <c r="F61" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="G61" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -4160,18 +4701,18 @@
         <v>-77.377323099999998</v>
       </c>
       <c r="F62" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="G62" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -4183,18 +4724,18 @@
         <v>-77.380240000000001</v>
       </c>
       <c r="F63" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="G63" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -4206,18 +4747,18 @@
         <v>-77.466695999999999</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G64" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -4229,18 +4770,18 @@
         <v>-77.379420300000007</v>
       </c>
       <c r="F65" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="G65" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -4252,10 +4793,10 @@
         <v>-77.562668000000002</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="G66" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -4309,7 +4850,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -4345,15 +4886,15 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4365,21 +4906,21 @@
         <v>-77.448892999999998</v>
       </c>
       <c r="F2" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="G2" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="H2" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -4391,21 +4932,21 @@
         <v>-77.558838699999995</v>
       </c>
       <c r="F3" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="G3" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -4417,21 +4958,21 @@
         <v>-77.234896500000005</v>
       </c>
       <c r="F4" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="G4" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -4443,21 +4984,21 @@
         <v>-77.547101999999995</v>
       </c>
       <c r="F5" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="G5" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -4469,18 +5010,18 @@
         <v>-77.448892999999998</v>
       </c>
       <c r="F6" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="G6" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B7" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -4492,21 +5033,21 @@
         <v>-77.377323099999998</v>
       </c>
       <c r="F7" t="s">
+        <v>263</v>
+      </c>
+      <c r="G7" t="s">
+        <v>288</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>277</v>
-      </c>
-      <c r="G7" t="s">
-        <v>302</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B8" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -4518,21 +5059,21 @@
         <v>-77.477527100000003</v>
       </c>
       <c r="F8" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="G8" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B9" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -4544,21 +5085,21 @@
         <v>-77.4392</v>
       </c>
       <c r="F9" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="G9" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B10" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -4570,21 +5111,21 @@
         <v>-77.412748199999996</v>
       </c>
       <c r="F10" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="G10" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="H10" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -4596,21 +5137,21 @@
         <v>-77.203404300000003</v>
       </c>
       <c r="F11" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="G11" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B12" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -4622,21 +5163,21 @@
         <v>-77.401802900000007</v>
       </c>
       <c r="F12" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="G12" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="H12" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B13" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -4648,21 +5189,21 @@
         <v>-77.385575399999993</v>
       </c>
       <c r="F13" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="G13" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B14" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -4674,21 +5215,21 @@
         <v>-77.347973999999994</v>
       </c>
       <c r="F14" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="G14" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B15" t="s">
         <v>264</v>
-      </c>
-      <c r="B15" t="s">
-        <v>278</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -4700,21 +5241,21 @@
         <v>-77.380240000000001</v>
       </c>
       <c r="F15" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="G15" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B16" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -4726,21 +5267,21 @@
         <v>-77.565303900000004</v>
       </c>
       <c r="F16" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="G16" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="H16" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -4752,21 +5293,21 @@
         <v>-77.547101999999995</v>
       </c>
       <c r="F17" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="G17" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="B18" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -4778,21 +5319,21 @@
         <v>-77.158857999999995</v>
       </c>
       <c r="F18" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="G18" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="H18" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="B19" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -4804,21 +5345,21 @@
         <v>-77.407484600000004</v>
       </c>
       <c r="F19" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="G19" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="B20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -4830,21 +5371,21 @@
         <v>-77.389587402343693</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="G20" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="B21" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -4856,21 +5397,21 @@
         <v>-77.466695999999999</v>
       </c>
       <c r="F21" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="G21" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="H21" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="B22" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -4882,149 +5423,149 @@
         <v>-77.471795599999993</v>
       </c>
       <c r="F22" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="G22" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="B23" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="B24" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B25" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B26" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B27" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="G27" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="H27" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B28" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="G28" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="H28" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B29" t="s">
+        <v>331</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>344</v>
+      </c>
+      <c r="G29" t="s">
         <v>345</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
-        <v>358</v>
-      </c>
-      <c r="G29" t="s">
-        <v>359</v>
-      </c>
       <c r="H29" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B30" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="G30" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -5077,15 +5618,15 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="32">
       <c r="A2" s="6" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5097,18 +5638,18 @@
         <v>-77.384056091308594</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="34.5" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -5120,18 +5661,18 @@
         <v>-77.368133799999995</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16">
       <c r="A4" s="6" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -5143,15 +5684,15 @@
         <v>-77.346993900000001</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32">
       <c r="A5" s="6" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5163,18 +5704,18 @@
         <v>-77.552453799999995</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="32">
       <c r="A6" s="6" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -5186,18 +5727,18 @@
         <v>-77.520797729492102</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="48">
       <c r="A7" s="6" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5209,18 +5750,18 @@
         <v>-77.310793799999999</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="32">
       <c r="A8" s="6" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -5232,18 +5773,18 @@
         <v>-77.149856567382798</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="32">
       <c r="A9" s="6" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="D9">
         <v>38.9978257</v>
@@ -5252,10 +5793,10 @@
         <v>-77.406757200000001</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5264,7 +5805,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="6" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B11" s="6"/>
     </row>
@@ -5658,6 +6199,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="cf6ddc61-6b1c-4d58-9daa-562ef749da72" xsi:nil="true"/>
@@ -5666,15 +6216,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5915,26 +6456,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3976ED70-E3F6-4CCF-93B3-12ADB5FE7646}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEA05EE-7518-4953-B638-950A17C44AF7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="d3dcd26c-518f-4103-85e3-288a7f67eda7"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cf6ddc61-6b1c-4d58-9daa-562ef749da72"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEA05EE-7518-4953-B638-950A17C44AF7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3976ED70-E3F6-4CCF-93B3-12ADB5FE7646}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d3dcd26c-518f-4103-85e3-288a7f67eda7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cf6ddc61-6b1c-4d58-9daa-562ef749da72"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>